<commit_message>
Add arduino code and DataSet xml code
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coco\Desktop\Exo low Ctrl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coco\Desktop\MultiServoController\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -924,7 +924,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>